<commit_message>
feat(Balancing): added Damage Type for each attack (Primary/Secondary). Changed values according to spread sheet.
</commit_message>
<xml_diff>
--- a/Balancing Sheet.xlsx
+++ b/Balancing Sheet.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\senpai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{645757AA-F452-4032-AB2B-D9F92F5378F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F001A4-838E-4807-A2DE-1484B3E30C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="37470" windowHeight="21840"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Balancing Sheet (2)" sheetId="2" r:id="rId1"/>
@@ -19,20 +19,33 @@
   <definedNames>
     <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">'Balancing Sheet (2)'!$A$1:$D$45</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Abfrage - Balancing Sheet" description="Verbindung mit der Abfrage 'Balancing Sheet' in der Arbeitsmappe." type="5" refreshedVersion="8" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Abfrage - Balancing Sheet" description="Verbindung mit der Abfrage 'Balancing Sheet' in der Arbeitsmappe." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Balancing Sheet&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Balancing Sheet]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
   <si>
     <t>,Player,Enemy,</t>
   </si>
@@ -224,9 +237,6 @@
   </si>
   <si>
     <t>80</t>
-  </si>
-  <si>
-    <t>90</t>
   </si>
   <si>
     <t>30</t>
@@ -286,7 +296,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -813,7 +823,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -822,6 +832,9 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -903,7 +916,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExterneDaten_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExterneDaten_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8" unboundColumnsRight="3">
     <queryTableFields count="7">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
@@ -919,16 +932,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Balancing_Sheet" displayName="Balancing_Sheet" ref="A1:G45" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Balancing_Sheet" displayName="Balancing_Sheet" ref="A1:G45" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G45" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="6"/>
-    <tableColumn id="2" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="3" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="4"/>
-    <tableColumn id="4" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="3"/>
-    <tableColumn id="5" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="1"/>
-    <tableColumn id="7" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1230,11 +1243,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P1:S28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,16 +1273,16 @@
         <v>41</v>
       </c>
       <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
         <v>79</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>80</v>
       </c>
-      <c r="G1" t="s">
-        <v>81</v>
-      </c>
       <c r="M1" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>43</v>
@@ -1299,7 +1312,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="M2" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N2" s="7">
         <f>B$3/$B14</f>
@@ -1331,7 +1344,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="M3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" ref="N3:O7" si="0">B$3/$B15</f>
@@ -1353,8 +1366,8 @@
       <c r="B4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>50</v>
+      <c r="C4" s="1">
+        <v>150</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>42</v>
@@ -1363,15 +1376,15 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="M4" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" si="0"/>
-        <v>5.5555555555555554</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="O4" s="7">
         <f t="shared" si="0"/>
-        <v>2.2222222222222223</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
@@ -1395,7 +1408,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="M5" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="0"/>
@@ -1427,7 +1440,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="M6" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" si="0"/>
@@ -1449,8 +1462,8 @@
       <c r="B7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>54</v>
+      <c r="C7" s="1">
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>42</v>
@@ -1459,7 +1472,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="M7" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" si="0"/>
@@ -1542,7 +1555,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="M10" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N10" s="7" t="s">
         <v>43</v>
@@ -1572,7 +1585,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="M11" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N11" s="5">
         <f>B$5/$C14</f>
@@ -1598,7 +1611,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="M12" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N12" s="5">
         <f t="shared" ref="N12:O16" si="1">B$5/$C15</f>
@@ -1618,7 +1631,7 @@
         <v>60</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>61</v>
@@ -1626,7 +1639,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="1"/>
       <c r="M13" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N13" s="5">
         <f t="shared" si="1"/>
@@ -1643,7 +1656,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>62</v>
@@ -1652,11 +1665,11 @@
         <v>56</v>
       </c>
       <c r="D14" s="3">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G14" s="1"/>
       <c r="M14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="1"/>
@@ -1673,20 +1686,20 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="3">
         <v>1.2</v>
       </c>
       <c r="G15" s="1"/>
       <c r="M15" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N15" s="5">
         <f t="shared" si="1"/>
@@ -1703,20 +1716,20 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
+      </c>
+      <c r="B16" s="8">
+        <v>75</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" s="2">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="G16" s="1"/>
       <c r="M16" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="1"/>
@@ -1733,16 +1746,16 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="2">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="G17" s="1"/>
       <c r="P17" s="5"/>
@@ -1752,16 +1765,16 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
@@ -1770,16 +1783,16 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="3">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
@@ -1811,7 +1824,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="M22" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N22" s="7" t="s">
         <v>43</v>
@@ -1828,15 +1841,15 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="M23" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N23" s="5">
         <f>B$4/($B14*$D14)</f>
-        <v>3</v>
+        <v>3.2727272727272725</v>
       </c>
       <c r="O23" s="5">
         <f>C$4/($B14*$D14)</f>
-        <v>1.6666666666666667</v>
+        <v>2.7272727272727271</v>
       </c>
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
@@ -1847,7 +1860,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="M24" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N24" s="5">
         <f t="shared" ref="N24:O28" si="2">B$4/($B15*$D15)</f>
@@ -1855,7 +1868,7 @@
       </c>
       <c r="O24" s="5">
         <f t="shared" si="2"/>
-        <v>1.0416666666666667</v>
+        <v>1.5625</v>
       </c>
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
@@ -1864,15 +1877,15 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M25" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N25" s="5">
         <f t="shared" si="2"/>
-        <v>1.1111111111111112</v>
+        <v>1.6</v>
       </c>
       <c r="O25" s="5">
         <f t="shared" si="2"/>
-        <v>0.61728395061728392</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
@@ -1881,15 +1894,15 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M26" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N26" s="5">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="O26" s="5">
         <f t="shared" si="2"/>
-        <v>1.1111111111111112</v>
+        <v>1.5</v>
       </c>
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
@@ -1898,15 +1911,15 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M27" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N27" s="5">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f>B$4/($B18*$D18)</f>
+        <v>12</v>
       </c>
       <c r="O27" s="5">
-        <f t="shared" si="2"/>
-        <v>3.3333333333333335</v>
+        <f>C$4/($B18*$D18)</f>
+        <v>10</v>
       </c>
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
@@ -1915,15 +1928,15 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M28" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N28" s="5">
         <f t="shared" si="2"/>
-        <v>2.4</v>
+        <v>3.4285714285714284</v>
       </c>
       <c r="O28" s="5">
         <f t="shared" si="2"/>
-        <v>1.3333333333333333</v>
+        <v>2.8571428571428572</v>
       </c>
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
@@ -1940,7 +1953,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A44"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
feat(Balancing): weapons now using the correct Damage Types
</commit_message>
<xml_diff>
--- a/Balancing Sheet.xlsx
+++ b/Balancing Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\senpai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F001A4-838E-4807-A2DE-1484B3E30C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6471A3-A218-42A2-92CD-ED38BDBAA9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="18015" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Balancing Sheet (2)" sheetId="2" r:id="rId1"/>
@@ -1246,8 +1246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1366,7 @@
       <c r="B4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="8">
         <v>150</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1462,7 +1462,7 @@
       <c r="B7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="8">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1755,7 +1755,7 @@
         <v>75</v>
       </c>
       <c r="D17" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G17" s="1"/>
       <c r="P17" s="5"/>
@@ -1898,11 +1898,11 @@
       </c>
       <c r="N26" s="5">
         <f t="shared" si="2"/>
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="O26" s="5">
         <f t="shared" si="2"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>

</xml_diff>

<commit_message>
fix(Balancing): fixed enemy max stagger
</commit_message>
<xml_diff>
--- a/Balancing Sheet.xlsx
+++ b/Balancing Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\senpai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6471A3-A218-42A2-92CD-ED38BDBAA9FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA1B77A-6B77-47C3-9DF6-B0FBB3B851CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="18015" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="81">
   <si>
     <t>,Player,Enemy,</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>Secondas until empty Stagger</t>
-  </si>
-  <si>
-    <t>18</t>
   </si>
   <si>
     <t>DMG</t>
@@ -1246,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,16 +1270,16 @@
         <v>41</v>
       </c>
       <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>79</v>
       </c>
-      <c r="G1" t="s">
-        <v>80</v>
-      </c>
       <c r="M1" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>43</v>
@@ -1312,7 +1309,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="M2" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N2" s="7">
         <f>B$3/$B14</f>
@@ -1344,7 +1341,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="M3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N3" s="7">
         <f t="shared" ref="N3:O7" si="0">B$3/$B15</f>
@@ -1376,7 +1373,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="M4" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N4" s="7">
         <f t="shared" si="0"/>
@@ -1408,7 +1405,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="M5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="0"/>
@@ -1430,8 +1427,8 @@
       <c r="B6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>54</v>
+      <c r="C6" s="8">
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>42</v>
@@ -1440,7 +1437,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="M6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N6" s="7">
         <f t="shared" si="0"/>
@@ -1472,7 +1469,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="M7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N7" s="7">
         <f t="shared" si="0"/>
@@ -1555,7 +1552,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="M10" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N10" s="7" t="s">
         <v>43</v>
@@ -1572,11 +1569,13 @@
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>54</v>
+      <c r="B11" s="1">
+        <f>B4/B6</f>
+        <v>18</v>
+      </c>
+      <c r="C11" s="1">
+        <f>C4/C6</f>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>42</v>
@@ -1585,7 +1584,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="M11" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N11" s="5">
         <f>B$5/$C14</f>
@@ -1611,7 +1610,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="M12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N12" s="5">
         <f t="shared" ref="N12:O16" si="1">B$5/$C15</f>
@@ -1628,18 +1627,18 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="1"/>
       <c r="M13" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N13" s="5">
         <f t="shared" si="1"/>
@@ -1656,10 +1655,10 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>56</v>
@@ -1669,7 +1668,7 @@
       </c>
       <c r="G14" s="1"/>
       <c r="M14" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N14" s="5">
         <f t="shared" si="1"/>
@@ -1686,20 +1685,20 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="D15" s="3">
         <v>1.2</v>
       </c>
       <c r="G15" s="1"/>
       <c r="M15" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N15" s="5">
         <f t="shared" si="1"/>
@@ -1716,20 +1715,20 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="8">
         <v>75</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" s="2">
         <v>1.5</v>
       </c>
       <c r="G16" s="1"/>
       <c r="M16" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="1"/>
@@ -1746,13 +1745,13 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D17" s="2">
         <v>3</v>
@@ -1765,10 +1764,10 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>56</v>
@@ -1783,13 +1782,13 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="3">
         <v>0.7</v>
@@ -1824,7 +1823,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="M22" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N22" s="7" t="s">
         <v>43</v>
@@ -1841,7 +1840,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="M23" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N23" s="5">
         <f>B$4/($B14*$D14)</f>
@@ -1860,7 +1859,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="M24" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N24" s="5">
         <f t="shared" ref="N24:O28" si="2">B$4/($B15*$D15)</f>
@@ -1877,7 +1876,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M25" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N25" s="5">
         <f t="shared" si="2"/>
@@ -1894,7 +1893,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M26" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N26" s="5">
         <f t="shared" si="2"/>
@@ -1911,7 +1910,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M27" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N27" s="5">
         <f>B$4/($B18*$D18)</f>
@@ -1928,7 +1927,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="M28" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N28" s="5">
         <f t="shared" si="2"/>

</xml_diff>